<commit_message>
add knowledge points to the mipiToRaw
</commit_message>
<xml_diff>
--- a/MipiToRaw/mipiToRawCal.xlsx
+++ b/MipiToRaw/mipiToRawCal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Fred\ISP\ISPAlgorithmStudy\MipiToRaw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB09A8C-B253-4BE9-BBA9-3949BBB23B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B2B1D6-8528-49C1-9A38-1647E4D5092E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,12 +224,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -237,6 +231,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -519,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="K10:AM19"/>
+  <dimension ref="K10:AZ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AB8" sqref="AB8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AW19" sqref="AW19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.875" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -531,146 +534,146 @@
     <col min="11" max="11" width="1.875" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="12.125" customWidth="1"/>
     <col min="13" max="28" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.5" customWidth="1"/>
+    <col min="29" max="29" width="2.375" customWidth="1"/>
     <col min="30" max="30" width="2.5" customWidth="1"/>
     <col min="31" max="38" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7" customWidth="1"/>
+    <col min="39" max="39" width="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="10" spans="12:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
-      <c r="AA10" s="15"/>
-      <c r="AB10" s="15"/>
-      <c r="AC10" s="15"/>
-      <c r="AD10" s="15"/>
-      <c r="AE10" s="15"/>
-      <c r="AF10" s="15"/>
-      <c r="AG10" s="15"/>
-      <c r="AH10" s="15"/>
-      <c r="AI10" s="15"/>
-      <c r="AJ10" s="15"/>
-      <c r="AK10" s="15"/>
-      <c r="AL10" s="15"/>
-      <c r="AM10" s="15"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="13"/>
+      <c r="AG10" s="13"/>
+      <c r="AH10" s="13"/>
+      <c r="AI10" s="13"/>
+      <c r="AJ10" s="13"/>
+      <c r="AK10" s="13"/>
+      <c r="AL10" s="13"/>
+      <c r="AM10" s="13"/>
     </row>
     <row r="11" spans="12:39" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L11" s="16" t="s">
+      <c r="L11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="14"/>
-      <c r="AB11" s="14"/>
-      <c r="AC11" s="14"/>
-      <c r="AD11" s="14"/>
-      <c r="AE11" s="14"/>
-      <c r="AF11" s="14"/>
-      <c r="AG11" s="14"/>
-      <c r="AH11" s="14"/>
-      <c r="AI11" s="14"/>
-      <c r="AJ11" s="14"/>
-      <c r="AK11" s="14"/>
-      <c r="AL11" s="14"/>
-      <c r="AM11" s="14"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="12"/>
+      <c r="AE11" s="12"/>
+      <c r="AF11" s="12"/>
+      <c r="AG11" s="12"/>
+      <c r="AH11" s="12"/>
+      <c r="AI11" s="12"/>
+      <c r="AJ11" s="12"/>
+      <c r="AK11" s="12"/>
+      <c r="AL11" s="12"/>
+      <c r="AM11" s="12"/>
     </row>
     <row r="12" spans="12:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L12" s="13" t="s">
+      <c r="L12" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="14"/>
-      <c r="AB12" s="14"/>
-      <c r="AC12" s="14"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="12"/>
+      <c r="AB12" s="12"/>
+      <c r="AC12" s="12"/>
       <c r="AD12" s="3"/>
-      <c r="AE12" s="13" t="s">
+      <c r="AE12" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="AF12" s="14"/>
-      <c r="AG12" s="14"/>
-      <c r="AH12" s="14"/>
-      <c r="AI12" s="14"/>
-      <c r="AJ12" s="14"/>
-      <c r="AK12" s="14"/>
-      <c r="AL12" s="14"/>
-      <c r="AM12" s="14"/>
+      <c r="AF12" s="12"/>
+      <c r="AG12" s="12"/>
+      <c r="AH12" s="12"/>
+      <c r="AI12" s="12"/>
+      <c r="AJ12" s="12"/>
+      <c r="AK12" s="12"/>
+      <c r="AL12" s="12"/>
+      <c r="AM12" s="12"/>
     </row>
     <row r="13" spans="12:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M13" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="12"/>
-      <c r="AB13" s="12"/>
+      <c r="M13" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
       <c r="AC13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="AD13" s="1"/>
-      <c r="AE13" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF13" s="12"/>
-      <c r="AG13" s="12"/>
-      <c r="AH13" s="12"/>
-      <c r="AI13" s="12"/>
-      <c r="AJ13" s="12"/>
-      <c r="AK13" s="12"/>
-      <c r="AL13" s="12"/>
+      <c r="AE13" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF13" s="15"/>
+      <c r="AG13" s="15"/>
+      <c r="AH13" s="15"/>
+      <c r="AI13" s="15"/>
+      <c r="AJ13" s="15"/>
+      <c r="AK13" s="15"/>
+      <c r="AL13" s="15"/>
       <c r="AM13" s="1" t="s">
         <v>2</v>
       </c>
@@ -960,7 +963,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="12:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="12:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L17" s="8">
         <f t="shared" si="1"/>
         <v>840</v>
@@ -1055,7 +1058,7 @@
         <v>D2</v>
       </c>
     </row>
-    <row r="18" spans="12:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="12:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -1112,40 +1115,90 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="12:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L19" s="14" t="s">
+    <row r="19" spans="12:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L19" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-      <c r="W19" s="14"/>
-      <c r="X19" s="14"/>
-      <c r="Y19" s="14"/>
-      <c r="Z19" s="14"/>
-      <c r="AA19" s="14"/>
-      <c r="AB19" s="14"/>
-      <c r="AC19" s="14"/>
-      <c r="AD19" s="14"/>
-      <c r="AE19" s="14"/>
-      <c r="AF19" s="14"/>
-      <c r="AG19" s="14"/>
-      <c r="AH19" s="14"/>
-      <c r="AI19" s="14"/>
-      <c r="AJ19" s="14"/>
-      <c r="AK19" s="14"/>
-      <c r="AL19" s="14"/>
-      <c r="AM19" s="14"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="12"/>
+      <c r="AA19" s="12"/>
+      <c r="AB19" s="12"/>
+      <c r="AC19" s="12"/>
+      <c r="AD19" s="12"/>
+      <c r="AE19" s="12"/>
+      <c r="AF19" s="12"/>
+      <c r="AG19" s="12"/>
+      <c r="AH19" s="12"/>
+      <c r="AI19" s="12"/>
+      <c r="AJ19" s="12"/>
+      <c r="AK19" s="12"/>
+      <c r="AL19" s="12"/>
+      <c r="AM19" s="12"/>
     </row>
+    <row r="21" spans="12:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="17"/>
+      <c r="V21" s="17"/>
+      <c r="W21" s="17"/>
+      <c r="X21" s="17"/>
+      <c r="Y21" s="17"/>
+      <c r="Z21" s="17"/>
+      <c r="AA21" s="17"/>
+      <c r="AB21" s="17"/>
+      <c r="AC21" s="17"/>
+      <c r="AD21" s="17"/>
+      <c r="AE21" s="17"/>
+      <c r="AF21" s="17"/>
+      <c r="AG21" s="17"/>
+      <c r="AH21" s="17"/>
+      <c r="AI21" s="17"/>
+      <c r="AJ21" s="17"/>
+      <c r="AK21" s="17"/>
+      <c r="AL21" s="17"/>
+      <c r="AM21" s="17"/>
+      <c r="AN21" s="17"/>
+      <c r="AO21" s="17"/>
+      <c r="AP21" s="17"/>
+      <c r="AQ21" s="17"/>
+      <c r="AR21" s="17"/>
+      <c r="AS21" s="17"/>
+      <c r="AT21" s="17"/>
+      <c r="AU21" s="17"/>
+      <c r="AV21" s="17"/>
+      <c r="AW21" s="17"/>
+      <c r="AX21" s="17"/>
+      <c r="AY21" s="17"/>
+      <c r="AZ21" s="17"/>
+    </row>
+    <row r="31" spans="12:52" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="12">
+    <mergeCell ref="AK21:AR21"/>
+    <mergeCell ref="AS21:AZ21"/>
+    <mergeCell ref="M21:T21"/>
+    <mergeCell ref="U21:AB21"/>
+    <mergeCell ref="AC21:AJ21"/>
     <mergeCell ref="L19:AM19"/>
     <mergeCell ref="L10:AM10"/>
     <mergeCell ref="L11:AM11"/>

</xml_diff>